<commit_message>
LITE-28124 Add parameters dependencies support for product operations
</commit_message>
<xml_diff>
--- a/tests/fixtures/params_sync.xlsx
+++ b/tests/fixtures/params_sync.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esovca00/PycharmProjects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B757ADAF-DBCE-CB45-8E1F-1407CEC80877}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA42ECC6-4A38-A642-AE75-FBD94DA601F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36180" yWindow="500" windowWidth="35840" windowHeight="20720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -180,13 +180,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>{
-    "constraints": {},
-    "hint": "I am the hint text",
-    "placeholder": "I am the placeholder text"
-}</t>
-  </si>
-  <si>
     <t>2020-10-13T01:24:49+00:00</t>
   </si>
   <si>
@@ -242,6 +235,25 @@
   </si>
   <si>
     <t>2020-11-27T08:37:16+00:00</t>
+  </si>
+  <si>
+    <t>{
+    "constraints": {
+        "dependency":{
+            "hidden": true,
+            "parameter": {
+                "id": "PRM-276-377-545-0008",
+                "name": "t0_o_email"
+            },
+            "required": true,
+            "values": [
+                "test@ex.com"
+            ]
+        }
+    },
+    "hint": "I am the hint text",
+    "placeholder": "I am the placeholder text"
+}</t>
   </si>
 </sst>
 </file>
@@ -757,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -847,13 +859,13 @@
         <v>24</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -937,19 +949,19 @@
     </row>
     <row r="2" spans="1:14" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>32</v>
@@ -958,7 +970,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" s="8" t="b">
         <v>1</v>
@@ -970,13 +982,13 @@
         <v>24</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="N2" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1060,28 +1072,28 @@
     </row>
     <row r="2" spans="1:14" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="H2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>24</v>
@@ -1093,13 +1105,13 @@
         <v>24</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="N2" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>